<commit_message>
Fixed audio out button listener
</commit_message>
<xml_diff>
--- a/CheckSamples.xlsx
+++ b/CheckSamples.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>freqOfTone</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>numSamples</t>
+  </si>
+  <si>
+    <t>sample[0]</t>
   </si>
 </sst>
 </file>
@@ -379,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -390,7 +393,7 @@
     <col min="1" max="1" width="15.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -398,7 +401,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -406,7 +409,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -414,7 +417,7 @@
         <v>44100</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -423,13 +426,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <f>INT(0.5+B5*(B3/B1))</f>
         <v>1002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f>B8/($B$3/$B$1)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final changes before moving audio to separate thread
</commit_message>
<xml_diff>
--- a/CheckSamples.xlsx
+++ b/CheckSamples.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>freqOfTone</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>sample[0]</t>
+  </si>
+  <si>
+    <t>sample[1]</t>
   </si>
 </sst>
 </file>
@@ -382,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -447,6 +450,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <f>INT(32767*SIN(2*PI()*B9/($B$3/$B$1)))</f>
+        <v>6126</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>